<commit_message>
PCA and regression solving with oultier
</commit_message>
<xml_diff>
--- a/data/calculatingTerminalIQR.xlsx
+++ b/data/calculatingTerminalIQR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/flight-python-scripts-winter2020/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/ocotillo-research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60EC2BD8-208F-7246-9F8B-28FBA81CB2DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C37D1D5-16F2-FF4B-98A6-940B939AF936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="28040" windowHeight="16740" xr2:uid="{7AB34404-82E0-0A4E-8A29-9001BB80DDD5}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16600" xr2:uid="{7AB34404-82E0-0A4E-8A29-9001BB80DDD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B34DF1-D27E-7E4A-8EC7-EE5BBE7A23F3}">
   <dimension ref="A1:BB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BB13" sqref="BB13"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>

</xml_diff>